<commit_message>
burn down chart, uppdatering av stylesheet och script för karaktärsbladet
</commit_message>
<xml_diff>
--- a/burntdown_chart.xlsx
+++ b/burntdown_chart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="2980" windowWidth="24960" windowHeight="14740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
     <t>Weeks</t>
   </si>
   <si>
-    <t>time spent</t>
+    <t>Difference</t>
   </si>
 </sst>
 </file>
@@ -167,7 +167,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Burnt down chart</a:t>
+              <a:t>Burndown chart</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -383,11 +383,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-709597808"/>
-        <c:axId val="-709585232"/>
+        <c:axId val="-1823691200"/>
+        <c:axId val="-1823802368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-709597808"/>
+        <c:axId val="-1823691200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -446,7 +446,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-709585232"/>
+        <c:crossAx val="-1823802368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -454,7 +454,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-709585232"/>
+        <c:axId val="-1823802368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="880.0"/>
@@ -514,7 +514,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-709597808"/>
+        <c:crossAx val="-1823691200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1449,7 +1449,7 @@
   <dimension ref="B4:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1493,7 +1493,7 @@
         <v>880</v>
       </c>
       <c r="E6">
-        <f>D6-C6</f>
+        <f t="shared" ref="E6:E11" si="0">D6-C6</f>
         <v>74</v>
       </c>
     </row>
@@ -1508,7 +1508,7 @@
         <v>849</v>
       </c>
       <c r="E7">
-        <f>D7-C7</f>
+        <f t="shared" si="0"/>
         <v>117</v>
       </c>
     </row>
@@ -1523,7 +1523,7 @@
         <v>807</v>
       </c>
       <c r="E8">
-        <f>D8-C8</f>
+        <f t="shared" si="0"/>
         <v>149</v>
       </c>
     </row>
@@ -1538,7 +1538,7 @@
         <v>671</v>
       </c>
       <c r="E9">
-        <f>D9-C9</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
@@ -1550,7 +1550,7 @@
         <v>510</v>
       </c>
       <c r="E10">
-        <f>D10-C10</f>
+        <f t="shared" si="0"/>
         <v>-510</v>
       </c>
     </row>
@@ -1562,7 +1562,7 @@
         <v>436</v>
       </c>
       <c r="E11">
-        <f>D11-C11</f>
+        <f t="shared" si="0"/>
         <v>-436</v>
       </c>
     </row>
@@ -1574,7 +1574,7 @@
         <v>362</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:E18" si="0">D12-C12</f>
+        <f t="shared" ref="E12:E18" si="1">D12-C12</f>
         <v>-362</v>
       </c>
     </row>
@@ -1586,7 +1586,7 @@
         <v>288</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-288</v>
       </c>
     </row>
@@ -1598,7 +1598,7 @@
         <v>214</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-214</v>
       </c>
     </row>
@@ -1610,7 +1610,7 @@
         <v>140</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-140</v>
       </c>
     </row>
@@ -1622,7 +1622,7 @@
         <v>66</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-66</v>
       </c>
     </row>
@@ -1634,7 +1634,7 @@
         <v>-8</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -1646,7 +1646,7 @@
         <v>-82</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>82</v>
       </c>
     </row>

</xml_diff>